<commit_message>
-Fix the BOM and some parts attributes
</commit_message>
<xml_diff>
--- a/H19R00/Released/BOM/H19R00.xlsx
+++ b/H19R00/Released/BOM/H19R00.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\HEXABITZ\Modules\Hardware\Modules Hardware Design\H19R0x-Hardware\H19R00\Released\BOM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Moazzen\Pictures\H19R00_11Oct2023\H19R00\Released\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56285C09-25DF-41F2-BF8C-1DBBDD681ACD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B315797-38F0-450E-B258-2998354B4B44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="255" windowWidth="19440" windowHeight="14880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="H19R00" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="144525"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="230">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="232">
   <si>
     <t>Description</t>
   </si>
@@ -589,9 +589,6 @@
     <t>RC0603FR-0710KL</t>
   </si>
   <si>
-    <t>CAP CER 470nF 100V X7R 0603</t>
-  </si>
-  <si>
     <t>CAP CER 0603 10nF 100V X7R</t>
   </si>
   <si>
@@ -716,13 +713,22 @@
   </si>
   <si>
     <t>https://octopart.com/apz0609470m050r-kyocera+avx-126722489?r=sp</t>
+  </si>
+  <si>
+    <t>https://octopart.com/search?q=C1608X5R1H474K080AB&amp;currency=USD&amp;specs=0</t>
+  </si>
+  <si>
+    <t>C1608X5R1H474K080AB</t>
+  </si>
+  <si>
+    <t>CAP CER 470nF 50V X5R 0603</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="31" x14ac:knownFonts="1">
+  <fonts count="30" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -762,12 +768,6 @@
       <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="28"/>
-      <name val="Trebuchet MS"/>
-      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -1321,49 +1321,49 @@
   <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="6" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="7" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="7" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="8" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="7" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="8" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="13" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="13" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="26" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="26" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="26" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="26" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="26" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="26" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="27" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="26" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="26" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="26" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="26" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="26" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="26" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1371,55 +1371,63 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="5" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="5" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="28" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="27" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="34" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="29" fillId="0" borderId="1" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1442,17 +1450,8 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="34" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="30" fillId="0" borderId="1" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="43">
@@ -1468,12 +1467,12 @@
     <cellStyle name="40% - Accent4" xfId="29" builtinId="43" customBuiltin="1"/>
     <cellStyle name="40% - Accent5" xfId="32" builtinId="47" customBuiltin="1"/>
     <cellStyle name="40% - Accent6" xfId="35" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60% - Accent1 2" xfId="37" xr:uid="{B25A1A21-3695-4D6C-A4C9-7B0E99729476}"/>
-    <cellStyle name="60% - Accent2 2" xfId="38" xr:uid="{980E3239-00C3-405C-9107-561A2CE11DE8}"/>
-    <cellStyle name="60% - Accent3 2" xfId="39" xr:uid="{5245F621-01EC-41AF-9137-03B1352287E4}"/>
-    <cellStyle name="60% - Accent4 2" xfId="40" xr:uid="{6F6DBE3A-B7DF-4FD4-BA36-56BD43E25716}"/>
-    <cellStyle name="60% - Accent5 2" xfId="41" xr:uid="{7E652C67-5ABE-49B3-989B-F24FCC7A0D38}"/>
-    <cellStyle name="60% - Accent6 2" xfId="42" xr:uid="{E4AE1A21-CBAE-44D5-A978-AE9BE04AB7BF}"/>
+    <cellStyle name="60% - Accent1 2" xfId="37" xr:uid="{00000000-0005-0000-0000-00000C000000}"/>
+    <cellStyle name="60% - Accent2 2" xfId="38" xr:uid="{00000000-0005-0000-0000-00000D000000}"/>
+    <cellStyle name="60% - Accent3 2" xfId="39" xr:uid="{00000000-0005-0000-0000-00000E000000}"/>
+    <cellStyle name="60% - Accent4 2" xfId="40" xr:uid="{00000000-0005-0000-0000-00000F000000}"/>
+    <cellStyle name="60% - Accent5 2" xfId="41" xr:uid="{00000000-0005-0000-0000-000010000000}"/>
+    <cellStyle name="60% - Accent6 2" xfId="42" xr:uid="{00000000-0005-0000-0000-000011000000}"/>
     <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
     <cellStyle name="Accent2" xfId="21" builtinId="33" customBuiltin="1"/>
     <cellStyle name="Accent3" xfId="24" builtinId="37" customBuiltin="1"/>
@@ -1492,7 +1491,7 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Neutral 2" xfId="36" xr:uid="{232CC50A-634F-4D19-A2A6-1BA4C8F85397}"/>
+    <cellStyle name="Neutral 2" xfId="36" xr:uid="{00000000-0005-0000-0000-000024000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
     <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
@@ -1616,7 +1615,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -1668,7 +1667,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -1872,8 +1871,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:G56"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A37" sqref="A37"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1894,8 +1893,7 @@
         <v>13</v>
       </c>
       <c r="D2" s="8"/>
-      <c r="E2" s="10"/>
-      <c r="F2" s="14" t="s">
+      <c r="E2" s="30" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1905,8 +1903,8 @@
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
-      <c r="F3" s="11"/>
-      <c r="G3" s="12"/>
+      <c r="F3" s="10"/>
+      <c r="G3" s="11"/>
     </row>
     <row r="4" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
@@ -1918,11 +1916,11 @@
       <c r="C4" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="21">
+      <c r="D4" s="23">
         <v>0</v>
       </c>
-      <c r="E4" s="21"/>
-      <c r="F4" s="21"/>
+      <c r="E4" s="23"/>
+      <c r="F4" s="23"/>
       <c r="G4" s="2"/>
     </row>
     <row r="5" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
@@ -1935,11 +1933,11 @@
       <c r="C5" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="22">
+      <c r="D5" s="24">
         <v>45209</v>
       </c>
-      <c r="E5" s="23"/>
-      <c r="F5" s="24"/>
+      <c r="E5" s="25"/>
+      <c r="F5" s="26"/>
       <c r="G5" s="2"/>
     </row>
     <row r="6" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
@@ -1952,9 +1950,9 @@
       <c r="C6" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D6" s="25"/>
-      <c r="E6" s="26"/>
-      <c r="F6" s="27"/>
+      <c r="D6" s="27"/>
+      <c r="E6" s="28"/>
+      <c r="F6" s="29"/>
       <c r="G6" s="2"/>
     </row>
     <row r="8" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
@@ -1964,10 +1962,10 @@
       <c r="B8" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C8" s="13" t="s">
+      <c r="C8" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="D8" s="13" t="s">
+      <c r="D8" s="12" t="s">
         <v>5</v>
       </c>
       <c r="E8" s="3" t="s">
@@ -1978,956 +1976,962 @@
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="28" t="s">
+      <c r="A9" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="B9" s="15" t="s">
+      <c r="B9" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="C9" s="15" t="s">
+      <c r="C9" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="D9" s="15" t="s">
+      <c r="D9" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="E9" s="29" t="s">
+      <c r="E9" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="F9" s="16">
+      <c r="F9" s="14">
         <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="28" t="s">
+      <c r="A10" s="19" t="s">
         <v>67</v>
       </c>
-      <c r="B10" s="15" t="s">
+      <c r="B10" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="C10" s="15" t="s">
+      <c r="C10" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="D10" s="15" t="s">
+      <c r="D10" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="E10" s="29" t="s">
+      <c r="E10" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="F10" s="16">
+      <c r="F10" s="14">
         <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="28" t="s">
+      <c r="A11" s="19" t="s">
         <v>157</v>
       </c>
-      <c r="B11" s="15" t="s">
+      <c r="B11" s="13" t="s">
         <v>158</v>
       </c>
-      <c r="C11" s="19">
+      <c r="C11" s="17">
         <v>691213710002</v>
       </c>
-      <c r="D11" s="15" t="s">
+      <c r="D11" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="E11" s="30" t="s">
+      <c r="E11" s="21" t="s">
+        <v>188</v>
+      </c>
+      <c r="F11" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="19" t="s">
+        <v>159</v>
+      </c>
+      <c r="B12" s="13" t="s">
+        <v>160</v>
+      </c>
+      <c r="C12" s="17">
+        <v>691213710003</v>
+      </c>
+      <c r="D12" s="13" t="s">
+        <v>161</v>
+      </c>
+      <c r="E12" s="21" t="s">
         <v>189</v>
       </c>
-      <c r="F11" s="15">
+      <c r="F12" s="13">
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="28" t="s">
-        <v>159</v>
-      </c>
-      <c r="B12" s="15" t="s">
-        <v>160</v>
-      </c>
-      <c r="C12" s="19">
-        <v>691213710003</v>
-      </c>
-      <c r="D12" s="15" t="s">
-        <v>161</v>
-      </c>
-      <c r="E12" s="30" t="s">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="19" t="s">
+        <v>129</v>
+      </c>
+      <c r="B13" s="13" t="s">
+        <v>130</v>
+      </c>
+      <c r="C13" s="17" t="s">
+        <v>131</v>
+      </c>
+      <c r="D13" s="13" t="s">
+        <v>132</v>
+      </c>
+      <c r="E13" s="21" t="s">
         <v>190</v>
       </c>
-      <c r="F12" s="15">
+      <c r="F13" s="13">
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="28" t="s">
-        <v>129</v>
-      </c>
-      <c r="B13" s="15" t="s">
-        <v>130</v>
-      </c>
-      <c r="C13" s="19" t="s">
-        <v>131</v>
-      </c>
-      <c r="D13" s="15" t="s">
-        <v>132</v>
-      </c>
-      <c r="E13" s="30" t="s">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="19" t="s">
+        <v>133</v>
+      </c>
+      <c r="B14" s="13" t="s">
+        <v>134</v>
+      </c>
+      <c r="C14" s="17" t="s">
+        <v>135</v>
+      </c>
+      <c r="D14" s="13" t="s">
+        <v>136</v>
+      </c>
+      <c r="E14" s="21" t="s">
         <v>191</v>
       </c>
-      <c r="F13" s="15">
+      <c r="F14" s="13">
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="28" t="s">
-        <v>133</v>
-      </c>
-      <c r="B14" s="15" t="s">
-        <v>134</v>
-      </c>
-      <c r="C14" s="19" t="s">
-        <v>135</v>
-      </c>
-      <c r="D14" s="15" t="s">
-        <v>136</v>
-      </c>
-      <c r="E14" s="30" t="s">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="19" t="s">
+        <v>71</v>
+      </c>
+      <c r="B15" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="C15" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="D15" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="E15" s="22" t="s">
+        <v>66</v>
+      </c>
+      <c r="F15" s="14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" s="18" customFormat="1" ht="29.4" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="19" t="s">
+        <v>72</v>
+      </c>
+      <c r="B16" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="C16" s="17" t="s">
+        <v>78</v>
+      </c>
+      <c r="D16" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="E16" s="21" t="s">
         <v>192</v>
       </c>
-      <c r="F14" s="15">
+      <c r="F16" s="13">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A17" s="19" t="s">
+        <v>84</v>
+      </c>
+      <c r="B17" s="13" t="s">
+        <v>85</v>
+      </c>
+      <c r="C17" s="17" t="s">
+        <v>86</v>
+      </c>
+      <c r="D17" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="E17" s="21" t="s">
+        <v>193</v>
+      </c>
+      <c r="F17" s="13">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="19" t="s">
+        <v>148</v>
+      </c>
+      <c r="B18" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="C18" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="D18" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="E18" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="F18" s="14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="19" t="s">
+        <v>107</v>
+      </c>
+      <c r="B19" s="13" t="s">
+        <v>108</v>
+      </c>
+      <c r="C19" s="17" t="s">
+        <v>109</v>
+      </c>
+      <c r="D19" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="E19" s="21" t="s">
+        <v>194</v>
+      </c>
+      <c r="F19" s="13">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="19" t="s">
+        <v>117</v>
+      </c>
+      <c r="B20" s="13" t="s">
+        <v>118</v>
+      </c>
+      <c r="C20" s="17" t="s">
+        <v>119</v>
+      </c>
+      <c r="D20" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="E20" s="21" t="s">
+        <v>195</v>
+      </c>
+      <c r="F20" s="13">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A21" s="19" t="s">
+        <v>123</v>
+      </c>
+      <c r="B21" s="13" t="s">
+        <v>124</v>
+      </c>
+      <c r="C21" s="17" t="s">
+        <v>125</v>
+      </c>
+      <c r="D21" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="E21" s="21" t="s">
+        <v>196</v>
+      </c>
+      <c r="F21" s="13">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="19" t="s">
+        <v>90</v>
+      </c>
+      <c r="B22" s="15" t="s">
+        <v>185</v>
+      </c>
+      <c r="C22" s="15" t="s">
+        <v>186</v>
+      </c>
+      <c r="D22" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="E22" s="20" t="s">
+        <v>197</v>
+      </c>
+      <c r="F22" s="14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="19" t="s">
+        <v>80</v>
+      </c>
+      <c r="B23" s="13" t="s">
+        <v>81</v>
+      </c>
+      <c r="C23" s="17" t="s">
+        <v>82</v>
+      </c>
+      <c r="D23" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="E23" s="21" t="s">
+        <v>198</v>
+      </c>
+      <c r="F23" s="13">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A24" s="19" t="s">
+        <v>97</v>
+      </c>
+      <c r="B24" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="C24" s="17" t="s">
+        <v>99</v>
+      </c>
+      <c r="D24" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="E24" s="21" t="s">
+        <v>199</v>
+      </c>
+      <c r="F24" s="13">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="19" t="s">
+        <v>105</v>
+      </c>
+      <c r="B25" s="13" t="s">
+        <v>106</v>
+      </c>
+      <c r="C25" s="17" t="s">
+        <v>220</v>
+      </c>
+      <c r="D25" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="E25" s="21" t="s">
+        <v>225</v>
+      </c>
+      <c r="F25" s="13">
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="28" t="s">
-        <v>71</v>
-      </c>
-      <c r="B15" s="15" t="s">
-        <v>64</v>
-      </c>
-      <c r="C15" s="15" t="s">
-        <v>65</v>
-      </c>
-      <c r="D15" s="15" t="s">
-        <v>31</v>
-      </c>
-      <c r="E15" s="31" t="s">
-        <v>66</v>
-      </c>
-      <c r="F15" s="16">
+    <row r="26" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A26" s="19" t="s">
+        <v>137</v>
+      </c>
+      <c r="B26" s="13" t="s">
+        <v>138</v>
+      </c>
+      <c r="C26" s="17" t="s">
+        <v>139</v>
+      </c>
+      <c r="D26" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="E26" s="21" t="s">
+        <v>200</v>
+      </c>
+      <c r="F26" s="13">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="19" t="s">
+        <v>87</v>
+      </c>
+      <c r="B27" s="13" t="s">
+        <v>88</v>
+      </c>
+      <c r="C27" s="17" t="s">
+        <v>89</v>
+      </c>
+      <c r="D27" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="E27" s="21" t="s">
+        <v>201</v>
+      </c>
+      <c r="F27" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="19" t="s">
+        <v>102</v>
+      </c>
+      <c r="B28" s="13" t="s">
+        <v>103</v>
+      </c>
+      <c r="C28" s="17" t="s">
+        <v>104</v>
+      </c>
+      <c r="D28" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="E28" s="21" t="s">
+        <v>202</v>
+      </c>
+      <c r="F28" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A29" s="19" t="s">
+        <v>69</v>
+      </c>
+      <c r="B29" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="C29" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="D29" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="E29" s="20" t="s">
+        <v>62</v>
+      </c>
+      <c r="F29" s="14">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" s="19" t="s">
+        <v>162</v>
+      </c>
+      <c r="B30" s="13" t="s">
+        <v>163</v>
+      </c>
+      <c r="C30" s="17" t="s">
+        <v>164</v>
+      </c>
+      <c r="D30" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="E30" s="21" t="s">
+        <v>203</v>
+      </c>
+      <c r="F30" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" s="19" t="s">
+        <v>126</v>
+      </c>
+      <c r="B31" s="13" t="s">
+        <v>127</v>
+      </c>
+      <c r="C31" s="17" t="s">
+        <v>128</v>
+      </c>
+      <c r="D31" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="E31" s="21" t="s">
+        <v>204</v>
+      </c>
+      <c r="F31" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" s="19" t="s">
+        <v>149</v>
+      </c>
+      <c r="B32" s="13" t="s">
+        <v>150</v>
+      </c>
+      <c r="C32" s="17" t="s">
+        <v>151</v>
+      </c>
+      <c r="D32" s="13" t="s">
+        <v>143</v>
+      </c>
+      <c r="E32" s="21" t="s">
+        <v>205</v>
+      </c>
+      <c r="F32" s="13">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" s="19" t="s">
+        <v>140</v>
+      </c>
+      <c r="B33" s="13" t="s">
+        <v>141</v>
+      </c>
+      <c r="C33" s="17" t="s">
+        <v>142</v>
+      </c>
+      <c r="D33" s="13" t="s">
+        <v>143</v>
+      </c>
+      <c r="E33" s="21" t="s">
+        <v>206</v>
+      </c>
+      <c r="F33" s="13">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" s="19" t="s">
+        <v>110</v>
+      </c>
+      <c r="B34" s="13" t="s">
+        <v>111</v>
+      </c>
+      <c r="C34" s="17" t="s">
+        <v>112</v>
+      </c>
+      <c r="D34" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="E34" s="21" t="s">
+        <v>207</v>
+      </c>
+      <c r="F34" s="13">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" s="19" t="s">
+        <v>120</v>
+      </c>
+      <c r="B35" s="13" t="s">
+        <v>121</v>
+      </c>
+      <c r="C35" s="17" t="s">
+        <v>122</v>
+      </c>
+      <c r="D35" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="E35" s="21" t="s">
+        <v>208</v>
+      </c>
+      <c r="F35" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" s="19" t="s">
+        <v>91</v>
+      </c>
+      <c r="B36" s="13" t="s">
+        <v>187</v>
+      </c>
+      <c r="C36" s="17" t="s">
+        <v>92</v>
+      </c>
+      <c r="D36" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="E36" s="21" t="s">
+        <v>209</v>
+      </c>
+      <c r="F36" s="13">
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:7" s="20" customFormat="1" ht="29.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="28" t="s">
-        <v>72</v>
-      </c>
-      <c r="B16" s="15" t="s">
-        <v>73</v>
-      </c>
-      <c r="C16" s="19" t="s">
-        <v>78</v>
-      </c>
-      <c r="D16" s="15" t="s">
-        <v>79</v>
-      </c>
-      <c r="E16" s="30" t="s">
-        <v>193</v>
-      </c>
-      <c r="F16" s="15">
+    <row r="37" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A37" s="19" t="s">
+        <v>183</v>
+      </c>
+      <c r="B37" s="13" t="s">
+        <v>210</v>
+      </c>
+      <c r="C37" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="D37" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="E37" s="20" t="s">
+        <v>211</v>
+      </c>
+      <c r="F37" s="14">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" s="19" t="s">
+        <v>100</v>
+      </c>
+      <c r="B38" s="13" t="s">
+        <v>101</v>
+      </c>
+      <c r="C38" s="17" t="s">
+        <v>221</v>
+      </c>
+      <c r="D38" s="13" t="s">
+        <v>222</v>
+      </c>
+      <c r="E38" s="21" t="s">
+        <v>226</v>
+      </c>
+      <c r="F38" s="13">
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A17" s="28" t="s">
-        <v>84</v>
-      </c>
-      <c r="B17" s="15" t="s">
-        <v>85</v>
-      </c>
-      <c r="C17" s="19" t="s">
-        <v>86</v>
-      </c>
-      <c r="D17" s="15" t="s">
-        <v>83</v>
-      </c>
-      <c r="E17" s="30" t="s">
-        <v>194</v>
-      </c>
-      <c r="F17" s="15">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" s="19" t="s">
+        <v>152</v>
+      </c>
+      <c r="B39" s="13" t="s">
+        <v>231</v>
+      </c>
+      <c r="C39" s="17" t="s">
+        <v>230</v>
+      </c>
+      <c r="D39" s="13" t="s">
+        <v>147</v>
+      </c>
+      <c r="E39" s="21" t="s">
+        <v>229</v>
+      </c>
+      <c r="F39" s="13">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" s="19" t="s">
+        <v>54</v>
+      </c>
+      <c r="B40" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="C40" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="D40" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="E40" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="F40" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41" s="19" t="s">
+        <v>113</v>
+      </c>
+      <c r="B41" s="13" t="s">
+        <v>114</v>
+      </c>
+      <c r="C41" s="17" t="s">
+        <v>115</v>
+      </c>
+      <c r="D41" s="13" t="s">
+        <v>116</v>
+      </c>
+      <c r="E41" s="21" t="s">
+        <v>212</v>
+      </c>
+      <c r="F41" s="13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42" s="19" t="s">
+        <v>55</v>
+      </c>
+      <c r="B42" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="C42" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="D42" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="E42" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="F42" s="14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A43" s="19" t="s">
+        <v>93</v>
+      </c>
+      <c r="B43" s="13" t="s">
+        <v>94</v>
+      </c>
+      <c r="C43" s="17" t="s">
+        <v>95</v>
+      </c>
+      <c r="D43" s="13" t="s">
+        <v>96</v>
+      </c>
+      <c r="E43" s="21" t="s">
+        <v>213</v>
+      </c>
+      <c r="F43" s="13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44" s="19" t="s">
+        <v>155</v>
+      </c>
+      <c r="B44" s="13" t="s">
+        <v>156</v>
+      </c>
+      <c r="C44" s="17" t="s">
+        <v>223</v>
+      </c>
+      <c r="D44" s="13" t="s">
+        <v>96</v>
+      </c>
+      <c r="E44" s="21" t="s">
+        <v>227</v>
+      </c>
+      <c r="F44" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45" s="19" t="s">
+        <v>153</v>
+      </c>
+      <c r="B45" s="13" t="s">
+        <v>154</v>
+      </c>
+      <c r="C45" s="17" t="s">
+        <v>224</v>
+      </c>
+      <c r="D45" s="13" t="s">
+        <v>222</v>
+      </c>
+      <c r="E45" s="21" t="s">
+        <v>228</v>
+      </c>
+      <c r="F45" s="13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="B46" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="C46" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="D46" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="E46" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="F46" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A47" s="19" t="s">
+        <v>144</v>
+      </c>
+      <c r="B47" s="13" t="s">
+        <v>145</v>
+      </c>
+      <c r="C47" s="17" t="s">
+        <v>146</v>
+      </c>
+      <c r="D47" s="13" t="s">
+        <v>147</v>
+      </c>
+      <c r="E47" s="21" t="s">
+        <v>214</v>
+      </c>
+      <c r="F47" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A48" s="19" t="s">
+        <v>179</v>
+      </c>
+      <c r="B48" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="C48" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="D48" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="E48" s="20" t="s">
+        <v>215</v>
+      </c>
+      <c r="F48" s="14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A49" s="19" t="s">
+        <v>167</v>
+      </c>
+      <c r="B49" s="13" t="s">
+        <v>168</v>
+      </c>
+      <c r="C49" s="17" t="s">
+        <v>169</v>
+      </c>
+      <c r="D49" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="E49" s="21" t="s">
+        <v>170</v>
+      </c>
+      <c r="F49" s="13">
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="28" t="s">
-        <v>148</v>
-      </c>
-      <c r="B18" s="15" t="s">
-        <v>51</v>
-      </c>
-      <c r="C18" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="D18" s="17" t="s">
-        <v>17</v>
-      </c>
-      <c r="E18" s="29" t="s">
-        <v>33</v>
-      </c>
-      <c r="F18" s="16">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="28" t="s">
-        <v>107</v>
-      </c>
-      <c r="B19" s="15" t="s">
-        <v>108</v>
-      </c>
-      <c r="C19" s="19" t="s">
-        <v>109</v>
-      </c>
-      <c r="D19" s="15" t="s">
-        <v>83</v>
-      </c>
-      <c r="E19" s="30" t="s">
-        <v>195</v>
-      </c>
-      <c r="F19" s="15">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A50" s="19" t="s">
+        <v>171</v>
+      </c>
+      <c r="B50" s="13" t="s">
+        <v>172</v>
+      </c>
+      <c r="C50" s="17" t="s">
+        <v>173</v>
+      </c>
+      <c r="D50" s="13" t="s">
+        <v>174</v>
+      </c>
+      <c r="E50" s="21" t="s">
+        <v>216</v>
+      </c>
+      <c r="F50" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A51" s="19" t="s">
+        <v>70</v>
+      </c>
+      <c r="B51" s="13" t="s">
+        <v>74</v>
+      </c>
+      <c r="C51" s="17" t="s">
+        <v>75</v>
+      </c>
+      <c r="D51" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="E51" s="21" t="s">
+        <v>77</v>
+      </c>
+      <c r="F51" s="13">
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="28" t="s">
-        <v>117</v>
-      </c>
-      <c r="B20" s="15" t="s">
-        <v>118</v>
-      </c>
-      <c r="C20" s="19" t="s">
-        <v>119</v>
-      </c>
-      <c r="D20" s="15" t="s">
-        <v>83</v>
-      </c>
-      <c r="E20" s="30" t="s">
-        <v>196</v>
-      </c>
-      <c r="F20" s="15">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A21" s="28" t="s">
-        <v>123</v>
-      </c>
-      <c r="B21" s="15" t="s">
-        <v>124</v>
-      </c>
-      <c r="C21" s="19" t="s">
-        <v>125</v>
-      </c>
-      <c r="D21" s="15" t="s">
-        <v>83</v>
-      </c>
-      <c r="E21" s="30" t="s">
-        <v>197</v>
-      </c>
-      <c r="F21" s="15">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="28" t="s">
-        <v>90</v>
-      </c>
-      <c r="B22" s="17" t="s">
-        <v>185</v>
-      </c>
-      <c r="C22" s="17" t="s">
-        <v>186</v>
-      </c>
-      <c r="D22" s="15" t="s">
-        <v>83</v>
-      </c>
-      <c r="E22" s="29" t="s">
-        <v>198</v>
-      </c>
-      <c r="F22" s="16">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="28" t="s">
-        <v>80</v>
-      </c>
-      <c r="B23" s="15" t="s">
-        <v>81</v>
-      </c>
-      <c r="C23" s="19" t="s">
-        <v>82</v>
-      </c>
-      <c r="D23" s="15" t="s">
-        <v>83</v>
-      </c>
-      <c r="E23" s="30" t="s">
-        <v>199</v>
-      </c>
-      <c r="F23" s="15">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A24" s="28" t="s">
-        <v>97</v>
-      </c>
-      <c r="B24" s="15" t="s">
-        <v>98</v>
-      </c>
-      <c r="C24" s="19" t="s">
-        <v>99</v>
-      </c>
-      <c r="D24" s="15" t="s">
-        <v>83</v>
-      </c>
-      <c r="E24" s="30" t="s">
-        <v>200</v>
-      </c>
-      <c r="F24" s="15">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="28" t="s">
-        <v>105</v>
-      </c>
-      <c r="B25" s="15" t="s">
-        <v>106</v>
-      </c>
-      <c r="C25" s="19" t="s">
-        <v>221</v>
-      </c>
-      <c r="D25" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="E25" s="30" t="s">
-        <v>226</v>
-      </c>
-      <c r="F25" s="15">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A52" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="B52" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="C52" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="D52" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="E52" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="F52" s="14">
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A26" s="28" t="s">
-        <v>137</v>
-      </c>
-      <c r="B26" s="15" t="s">
-        <v>138</v>
-      </c>
-      <c r="C26" s="19" t="s">
-        <v>139</v>
-      </c>
-      <c r="D26" s="15" t="s">
-        <v>83</v>
-      </c>
-      <c r="E26" s="30" t="s">
-        <v>201</v>
-      </c>
-      <c r="F26" s="15">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="28" t="s">
-        <v>87</v>
-      </c>
-      <c r="B27" s="15" t="s">
-        <v>88</v>
-      </c>
-      <c r="C27" s="19" t="s">
-        <v>89</v>
-      </c>
-      <c r="D27" s="15" t="s">
-        <v>83</v>
-      </c>
-      <c r="E27" s="30" t="s">
-        <v>202</v>
-      </c>
-      <c r="F27" s="15">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A53" s="19" t="s">
+        <v>61</v>
+      </c>
+      <c r="B53" s="13" t="s">
+        <v>180</v>
+      </c>
+      <c r="C53" s="17" t="s">
+        <v>181</v>
+      </c>
+      <c r="D53" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="E53" s="21" t="s">
+        <v>182</v>
+      </c>
+      <c r="F53" s="13">
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="28" t="s">
-        <v>102</v>
-      </c>
-      <c r="B28" s="15" t="s">
-        <v>103</v>
-      </c>
-      <c r="C28" s="19" t="s">
-        <v>104</v>
-      </c>
-      <c r="D28" s="15" t="s">
-        <v>83</v>
-      </c>
-      <c r="E28" s="30" t="s">
-        <v>203</v>
-      </c>
-      <c r="F28" s="15">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A54" s="19" t="s">
+        <v>165</v>
+      </c>
+      <c r="B54" s="13" t="s">
+        <v>219</v>
+      </c>
+      <c r="C54" s="17" t="s">
+        <v>166</v>
+      </c>
+      <c r="D54" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="E54" s="21" t="s">
+        <v>217</v>
+      </c>
+      <c r="F54" s="13">
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A29" s="28" t="s">
-        <v>69</v>
-      </c>
-      <c r="B29" s="17" t="s">
-        <v>58</v>
-      </c>
-      <c r="C29" s="17" t="s">
-        <v>57</v>
-      </c>
-      <c r="D29" s="15" t="s">
-        <v>59</v>
-      </c>
-      <c r="E29" s="29" t="s">
-        <v>62</v>
-      </c>
-      <c r="F29" s="16">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="28" t="s">
-        <v>162</v>
-      </c>
-      <c r="B30" s="15" t="s">
-        <v>163</v>
-      </c>
-      <c r="C30" s="19" t="s">
-        <v>164</v>
-      </c>
-      <c r="D30" s="15" t="s">
-        <v>83</v>
-      </c>
-      <c r="E30" s="30" t="s">
-        <v>204</v>
-      </c>
-      <c r="F30" s="15">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A55" s="19" t="s">
+        <v>175</v>
+      </c>
+      <c r="B55" s="13" t="s">
+        <v>176</v>
+      </c>
+      <c r="C55" s="17" t="s">
+        <v>177</v>
+      </c>
+      <c r="D55" s="13" t="s">
+        <v>178</v>
+      </c>
+      <c r="E55" s="21" t="s">
+        <v>218</v>
+      </c>
+      <c r="F55" s="13">
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="28" t="s">
-        <v>126</v>
-      </c>
-      <c r="B31" s="15" t="s">
-        <v>127</v>
-      </c>
-      <c r="C31" s="19" t="s">
-        <v>128</v>
-      </c>
-      <c r="D31" s="15" t="s">
-        <v>83</v>
-      </c>
-      <c r="E31" s="30" t="s">
-        <v>205</v>
-      </c>
-      <c r="F31" s="15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="28" t="s">
-        <v>149</v>
-      </c>
-      <c r="B32" s="15" t="s">
-        <v>150</v>
-      </c>
-      <c r="C32" s="19" t="s">
-        <v>151</v>
-      </c>
-      <c r="D32" s="15" t="s">
-        <v>143</v>
-      </c>
-      <c r="E32" s="30" t="s">
-        <v>206</v>
-      </c>
-      <c r="F32" s="15">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="28" t="s">
-        <v>140</v>
-      </c>
-      <c r="B33" s="15" t="s">
-        <v>141</v>
-      </c>
-      <c r="C33" s="19" t="s">
-        <v>142</v>
-      </c>
-      <c r="D33" s="15" t="s">
-        <v>143</v>
-      </c>
-      <c r="E33" s="30" t="s">
-        <v>207</v>
-      </c>
-      <c r="F33" s="15">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="28" t="s">
-        <v>110</v>
-      </c>
-      <c r="B34" s="15" t="s">
-        <v>111</v>
-      </c>
-      <c r="C34" s="19" t="s">
-        <v>112</v>
-      </c>
-      <c r="D34" s="15" t="s">
-        <v>59</v>
-      </c>
-      <c r="E34" s="30" t="s">
-        <v>208</v>
-      </c>
-      <c r="F34" s="15">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="28" t="s">
-        <v>120</v>
-      </c>
-      <c r="B35" s="15" t="s">
-        <v>121</v>
-      </c>
-      <c r="C35" s="19" t="s">
-        <v>122</v>
-      </c>
-      <c r="D35" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="E35" s="30" t="s">
-        <v>209</v>
-      </c>
-      <c r="F35" s="15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="28" t="s">
-        <v>91</v>
-      </c>
-      <c r="B36" s="15" t="s">
-        <v>188</v>
-      </c>
-      <c r="C36" s="19" t="s">
-        <v>92</v>
-      </c>
-      <c r="D36" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="E36" s="30" t="s">
-        <v>210</v>
-      </c>
-      <c r="F36" s="15">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A37" s="28" t="s">
-        <v>183</v>
-      </c>
-      <c r="B37" s="15" t="s">
-        <v>211</v>
-      </c>
-      <c r="C37" s="15" t="s">
-        <v>56</v>
-      </c>
-      <c r="D37" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="E37" s="29" t="s">
-        <v>212</v>
-      </c>
-      <c r="F37" s="16">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" s="28" t="s">
-        <v>100</v>
-      </c>
-      <c r="B38" s="15" t="s">
-        <v>101</v>
-      </c>
-      <c r="C38" s="19" t="s">
-        <v>222</v>
-      </c>
-      <c r="D38" s="15" t="s">
-        <v>223</v>
-      </c>
-      <c r="E38" s="30" t="s">
-        <v>227</v>
-      </c>
-      <c r="F38" s="15">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" s="28" t="s">
-        <v>152</v>
-      </c>
-      <c r="B39" s="15" t="s">
-        <v>187</v>
-      </c>
-      <c r="C39" s="19"/>
-      <c r="D39" s="15"/>
-      <c r="E39" s="30"/>
-      <c r="F39" s="15">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" s="28" t="s">
-        <v>54</v>
-      </c>
-      <c r="B40" s="17" t="s">
-        <v>50</v>
-      </c>
-      <c r="C40" s="17" t="s">
-        <v>29</v>
-      </c>
-      <c r="D40" s="17" t="s">
-        <v>28</v>
-      </c>
-      <c r="E40" s="29" t="s">
-        <v>30</v>
-      </c>
-      <c r="F40" s="16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41" s="28" t="s">
-        <v>113</v>
-      </c>
-      <c r="B41" s="15" t="s">
-        <v>114</v>
-      </c>
-      <c r="C41" s="19" t="s">
-        <v>115</v>
-      </c>
-      <c r="D41" s="15" t="s">
-        <v>116</v>
-      </c>
-      <c r="E41" s="30" t="s">
-        <v>213</v>
-      </c>
-      <c r="F41" s="15">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A42" s="28" t="s">
-        <v>55</v>
-      </c>
-      <c r="B42" s="15" t="s">
-        <v>49</v>
-      </c>
-      <c r="C42" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="D42" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="E42" s="29" t="s">
-        <v>19</v>
-      </c>
-      <c r="F42" s="16">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A43" s="28" t="s">
-        <v>93</v>
-      </c>
-      <c r="B43" s="15" t="s">
-        <v>94</v>
-      </c>
-      <c r="C43" s="19" t="s">
-        <v>95</v>
-      </c>
-      <c r="D43" s="15" t="s">
-        <v>96</v>
-      </c>
-      <c r="E43" s="30" t="s">
-        <v>214</v>
-      </c>
-      <c r="F43" s="15">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A44" s="28" t="s">
-        <v>155</v>
-      </c>
-      <c r="B44" s="15" t="s">
-        <v>156</v>
-      </c>
-      <c r="C44" s="19" t="s">
-        <v>224</v>
-      </c>
-      <c r="D44" s="15" t="s">
-        <v>96</v>
-      </c>
-      <c r="E44" s="30" t="s">
-        <v>228</v>
-      </c>
-      <c r="F44" s="15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A45" s="28" t="s">
-        <v>153</v>
-      </c>
-      <c r="B45" s="15" t="s">
-        <v>154</v>
-      </c>
-      <c r="C45" s="19" t="s">
-        <v>225</v>
-      </c>
-      <c r="D45" s="15" t="s">
-        <v>223</v>
-      </c>
-      <c r="E45" s="30" t="s">
-        <v>229</v>
-      </c>
-      <c r="F45" s="15">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="28" t="s">
-        <v>34</v>
-      </c>
-      <c r="B46" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="C46" s="15" t="s">
-        <v>37</v>
-      </c>
-      <c r="D46" s="15" t="s">
-        <v>36</v>
-      </c>
-      <c r="E46" s="29" t="s">
-        <v>38</v>
-      </c>
-      <c r="F46" s="16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A47" s="28" t="s">
-        <v>144</v>
-      </c>
-      <c r="B47" s="15" t="s">
-        <v>145</v>
-      </c>
-      <c r="C47" s="19" t="s">
-        <v>146</v>
-      </c>
-      <c r="D47" s="15" t="s">
-        <v>147</v>
-      </c>
-      <c r="E47" s="30" t="s">
-        <v>215</v>
-      </c>
-      <c r="F47" s="15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A48" s="28" t="s">
-        <v>179</v>
-      </c>
-      <c r="B48" s="15" t="s">
-        <v>52</v>
-      </c>
-      <c r="C48" s="15" t="s">
-        <v>44</v>
-      </c>
-      <c r="D48" s="15" t="s">
-        <v>20</v>
-      </c>
-      <c r="E48" s="29" t="s">
-        <v>216</v>
-      </c>
-      <c r="F48" s="16">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A49" s="28" t="s">
-        <v>167</v>
-      </c>
-      <c r="B49" s="15" t="s">
-        <v>168</v>
-      </c>
-      <c r="C49" s="19" t="s">
-        <v>169</v>
-      </c>
-      <c r="D49" s="15" t="s">
-        <v>42</v>
-      </c>
-      <c r="E49" s="30" t="s">
-        <v>170</v>
-      </c>
-      <c r="F49" s="15">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A50" s="28" t="s">
-        <v>171</v>
-      </c>
-      <c r="B50" s="15" t="s">
-        <v>172</v>
-      </c>
-      <c r="C50" s="19" t="s">
-        <v>173</v>
-      </c>
-      <c r="D50" s="15" t="s">
-        <v>174</v>
-      </c>
-      <c r="E50" s="30" t="s">
-        <v>217</v>
-      </c>
-      <c r="F50" s="15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A51" s="28" t="s">
-        <v>70</v>
-      </c>
-      <c r="B51" s="15" t="s">
-        <v>74</v>
-      </c>
-      <c r="C51" s="19" t="s">
-        <v>75</v>
-      </c>
-      <c r="D51" s="15" t="s">
-        <v>76</v>
-      </c>
-      <c r="E51" s="30" t="s">
-        <v>77</v>
-      </c>
-      <c r="F51" s="15">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A52" s="28" t="s">
-        <v>40</v>
-      </c>
-      <c r="B52" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="C52" s="15" t="s">
-        <v>39</v>
-      </c>
-      <c r="D52" s="15" t="s">
-        <v>42</v>
-      </c>
-      <c r="E52" s="29" t="s">
-        <v>43</v>
-      </c>
-      <c r="F52" s="16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A53" s="28" t="s">
-        <v>61</v>
-      </c>
-      <c r="B53" s="15" t="s">
-        <v>180</v>
-      </c>
-      <c r="C53" s="19" t="s">
-        <v>181</v>
-      </c>
-      <c r="D53" s="15" t="s">
-        <v>42</v>
-      </c>
-      <c r="E53" s="30" t="s">
-        <v>182</v>
-      </c>
-      <c r="F53" s="15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A54" s="28" t="s">
-        <v>165</v>
-      </c>
-      <c r="B54" s="15" t="s">
-        <v>220</v>
-      </c>
-      <c r="C54" s="19" t="s">
-        <v>166</v>
-      </c>
-      <c r="D54" s="15" t="s">
-        <v>60</v>
-      </c>
-      <c r="E54" s="30" t="s">
-        <v>218</v>
-      </c>
-      <c r="F54" s="15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A55" s="28" t="s">
-        <v>175</v>
-      </c>
-      <c r="B55" s="15" t="s">
-        <v>176</v>
-      </c>
-      <c r="C55" s="19" t="s">
-        <v>177</v>
-      </c>
-      <c r="D55" s="15" t="s">
-        <v>178</v>
-      </c>
-      <c r="E55" s="30" t="s">
-        <v>219</v>
-      </c>
-      <c r="F55" s="15">
-        <v>1</v>
-      </c>
-    </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A56" s="28" t="s">
+      <c r="A56" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="B56" s="15" t="s">
+      <c r="B56" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="C56" s="15" t="s">
+      <c r="C56" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="D56" s="15" t="s">
+      <c r="D56" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="E56" s="29" t="s">
+      <c r="E56" s="20" t="s">
         <v>48</v>
       </c>
-      <c r="F56" s="18">
+      <c r="F56" s="16">
         <v>1</v>
       </c>
     </row>
@@ -2938,41 +2942,41 @@
     <mergeCell ref="D6:F6"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="E9" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="E18" r:id="rId2" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
-    <hyperlink ref="E10" r:id="rId3" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
-    <hyperlink ref="E51" r:id="rId4" xr:uid="{95C0407A-E167-4833-9ED7-3C750B98877C}"/>
-    <hyperlink ref="E15" r:id="rId5" xr:uid="{CB888211-6DC0-49D9-8658-FBC69849BEA7}"/>
-    <hyperlink ref="E16" r:id="rId6" xr:uid="{77272C6B-0867-4BD7-A5D2-1B02F4255E59}"/>
-    <hyperlink ref="E17" r:id="rId7" xr:uid="{8A50D1DD-457F-4AEB-A24B-5A65512685CD}"/>
-    <hyperlink ref="E19" r:id="rId8" xr:uid="{5B749BC3-D662-42C9-A8E2-D5812FB5024F}"/>
-    <hyperlink ref="E20" r:id="rId9" xr:uid="{98D861F0-6A23-48D6-8A68-06F3DF16A53A}"/>
-    <hyperlink ref="E21" r:id="rId10" xr:uid="{85C2C1E6-CF70-4B15-A12A-4DE602C11600}"/>
-    <hyperlink ref="E22" r:id="rId11" xr:uid="{7AA58F02-6D9F-4A52-A59C-E6B00FDD1ECC}"/>
-    <hyperlink ref="E23" r:id="rId12" xr:uid="{EA143E30-2353-4929-ACF0-6197DC0464F6}"/>
-    <hyperlink ref="E24" r:id="rId13" xr:uid="{E88E0100-5921-4D4A-833E-7C4376F76408}"/>
-    <hyperlink ref="E26" r:id="rId14" xr:uid="{1EA5403A-B1AC-40A3-B894-6699B55F624A}"/>
-    <hyperlink ref="E27" r:id="rId15" xr:uid="{5C622BC1-037C-4628-AF0C-D7D7C477DD90}"/>
-    <hyperlink ref="E28" r:id="rId16" xr:uid="{ACA56608-FE0B-49DA-9F13-127E79E662C6}"/>
-    <hyperlink ref="E29" r:id="rId17" xr:uid="{C4F8CF74-9595-4F3B-BA8F-CE5E80C38F95}"/>
-    <hyperlink ref="E30" r:id="rId18" xr:uid="{17AA8F0F-193F-4F85-AA4E-70D6658FEB41}"/>
-    <hyperlink ref="E31" r:id="rId19" xr:uid="{806AA5C8-1CB6-4249-9D27-7AD61819AC80}"/>
-    <hyperlink ref="E32" r:id="rId20" xr:uid="{70D5E1C4-1227-4347-BD35-CDF8EE79AB6E}"/>
-    <hyperlink ref="E33" r:id="rId21" xr:uid="{F80679AE-5105-4E2C-8D2E-936F0F7316B2}"/>
-    <hyperlink ref="E34" r:id="rId22" xr:uid="{1BE7AB42-2B86-4CD8-B6CE-3FDAB31916F8}"/>
-    <hyperlink ref="E35" r:id="rId23" xr:uid="{410C82E6-2391-4BC2-BEC0-0FCFB0854A14}"/>
-    <hyperlink ref="E36" r:id="rId24" xr:uid="{F4DB2891-7DAC-4308-9308-76DE7299C96D}"/>
-    <hyperlink ref="E37" r:id="rId25" xr:uid="{917B8A5E-2F8E-4424-B530-0B1EDA5F5637}"/>
-    <hyperlink ref="E40" r:id="rId26" xr:uid="{FA1A5661-B571-46F5-B7DA-E760F7B71936}"/>
-    <hyperlink ref="E41" r:id="rId27" xr:uid="{B59FCEE0-97DA-45C8-AA7A-5788DC149542}"/>
-    <hyperlink ref="E42" r:id="rId28" xr:uid="{E721CE20-801C-4D0D-9359-D941C0031087}"/>
-    <hyperlink ref="E46" r:id="rId29" xr:uid="{6F86676D-553E-4DF4-815F-3F05D774CC9A}"/>
-    <hyperlink ref="E47" r:id="rId30" xr:uid="{BB5FB233-96D6-41B1-AE3B-B3F233FB38C6}"/>
-    <hyperlink ref="E48" r:id="rId31" xr:uid="{4523F960-4912-4A07-BF54-69474F235C0E}"/>
-    <hyperlink ref="E49" r:id="rId32" xr:uid="{EBE602C1-D6F9-4645-8E83-1E7C631A39D1}"/>
-    <hyperlink ref="E50" r:id="rId33" xr:uid="{B802AB49-1F95-461F-9B5E-F441B7944223}"/>
-    <hyperlink ref="E54" r:id="rId34" xr:uid="{EE863B67-FC4E-4E1C-8342-ACA69E2D2C6F}"/>
-    <hyperlink ref="E43" r:id="rId35" xr:uid="{6E343E24-B194-44A3-8DAC-90F365E17FC7}"/>
+    <hyperlink ref="E9" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="E18" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="E10" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="E51" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="E15" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="E16" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="E17" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="E19" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="E20" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="E21" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="E22" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="E23" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="E24" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="E26" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="E27" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="E28" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="E29" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="E30" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="E31" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="E32" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="E33" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
+    <hyperlink ref="E34" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
+    <hyperlink ref="E35" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
+    <hyperlink ref="E36" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
+    <hyperlink ref="E37" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
+    <hyperlink ref="E40" r:id="rId26" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
+    <hyperlink ref="E41" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
+    <hyperlink ref="E42" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
+    <hyperlink ref="E46" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
+    <hyperlink ref="E47" r:id="rId30" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
+    <hyperlink ref="E48" r:id="rId31" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
+    <hyperlink ref="E49" r:id="rId32" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
+    <hyperlink ref="E50" r:id="rId33" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
+    <hyperlink ref="E54" r:id="rId34" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
+    <hyperlink ref="E43" r:id="rId35" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId36"/>

</xml_diff>

<commit_message>
-Before editing the layout
</commit_message>
<xml_diff>
--- a/H19R00/Released/BOM/H19R00.xlsx
+++ b/H19R00/Released/BOM/H19R00.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\HEXABITZ\Modules\Hardware\Modules Hardware Design\H19R0x-Hardware\H19R00\Released\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F75CA97A-849F-4F32-A7FA-A379DB63D6FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD7F8465-DB95-44FE-BC03-207A848C18E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="255" windowWidth="19440" windowHeight="14880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="H19R00" sheetId="1" r:id="rId1"/>
@@ -91,18 +91,9 @@
     <t>Vishay</t>
   </si>
   <si>
-    <t>PCB Header, Unshrouded, Thru 02 Straight Header, .101, AMPMODU Mod II Series</t>
-  </si>
-  <si>
     <t>TE Connectivity</t>
   </si>
   <si>
-    <t>87227-1</t>
-  </si>
-  <si>
-    <t>https://octopart.com/87227-1-te+connectivity-39512052?r=sp</t>
-  </si>
-  <si>
     <t>Conn Unshrouded Header HDR 3 POS 2.54mm Solder ST Top Entry Thru-Hole Carton</t>
   </si>
   <si>
@@ -722,13 +713,22 @@
   </si>
   <si>
     <t>https://octopart.com/c1608x5r1h474k080ab-tdk-26013511?r=sp</t>
+  </si>
+  <si>
+    <t>Headers &amp; Wire Housings Unshrouded 1 POS T/H</t>
+  </si>
+  <si>
+    <t>5-146280-1</t>
+  </si>
+  <si>
+    <t>https://octopart.com/5-146280-1-te+connectivity+%2F+amp-40259676?r=sp</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="31" x14ac:knownFonts="1">
+  <fonts count="30" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -925,18 +925,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="9"/>
-      <color theme="1"/>
-      <name val="Segoe UI Semibold"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color rgb="FF000000"/>
-      <name val="Segoe UI Semibold"/>
-      <family val="2"/>
-    </font>
-    <font>
       <u/>
       <sz val="9"/>
       <color theme="10"/>
@@ -944,12 +932,16 @@
       <family val="2"/>
     </font>
     <font>
-      <u/>
       <sz val="9"/>
-      <color theme="10"/>
-      <name val="Arial"/>
+      <color theme="1"/>
+      <name val="Segoe UI"/>
       <family val="2"/>
-      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="35">
@@ -1371,7 +1363,7 @@
     <xf numFmtId="0" fontId="25" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="25" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1407,34 +1399,16 @@
     <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="27" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="34" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="29" fillId="0" borderId="1" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="27" fillId="0" borderId="1" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1461,7 +1435,22 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="34" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="28" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1882,17 +1871,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:G56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C17" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E39" sqref="E39"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.69921875" customWidth="1"/>
-    <col min="2" max="2" width="70.59765625" customWidth="1"/>
-    <col min="3" max="3" width="21.59765625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.8984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="84" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="58.3984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.19921875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.5" style="1" customWidth="1"/>
+    <col min="5" max="5" width="67.3984375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.3984375" customWidth="1"/>
     <col min="7" max="7" width="49" customWidth="1"/>
   </cols>
@@ -1904,7 +1893,7 @@
         <v>13</v>
       </c>
       <c r="D2" s="8"/>
-      <c r="E2" s="23" t="s">
+      <c r="E2" s="17" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1927,11 +1916,11 @@
       <c r="C4" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="24">
+      <c r="D4" s="18">
         <v>0</v>
       </c>
-      <c r="E4" s="24"/>
-      <c r="F4" s="24"/>
+      <c r="E4" s="18"/>
+      <c r="F4" s="18"/>
       <c r="G4" s="2"/>
     </row>
     <row r="5" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
@@ -1939,16 +1928,16 @@
         <v>9</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="25">
+      <c r="D5" s="19">
         <v>45209</v>
       </c>
-      <c r="E5" s="26"/>
-      <c r="F5" s="27"/>
+      <c r="E5" s="20"/>
+      <c r="F5" s="21"/>
       <c r="G5" s="2"/>
     </row>
     <row r="6" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
@@ -1956,14 +1945,14 @@
         <v>10</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D6" s="28"/>
-      <c r="E6" s="29"/>
-      <c r="F6" s="30"/>
+      <c r="D6" s="22"/>
+      <c r="E6" s="23"/>
+      <c r="F6" s="24"/>
       <c r="G6" s="2"/>
     </row>
     <row r="8" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
@@ -1987,962 +1976,962 @@
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="19" t="s">
+      <c r="A9" s="26" t="s">
+        <v>60</v>
+      </c>
+      <c r="B9" s="25" t="s">
+        <v>229</v>
+      </c>
+      <c r="C9" s="25" t="s">
+        <v>230</v>
+      </c>
+      <c r="D9" s="25" t="s">
+        <v>21</v>
+      </c>
+      <c r="E9" s="15" t="s">
+        <v>231</v>
+      </c>
+      <c r="F9" s="27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="26" t="s">
+        <v>64</v>
+      </c>
+      <c r="B10" s="25" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" s="25" t="s">
+        <v>23</v>
+      </c>
+      <c r="D10" s="25" t="s">
+        <v>21</v>
+      </c>
+      <c r="E10" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="F10" s="27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="26" t="s">
+        <v>154</v>
+      </c>
+      <c r="B11" s="25" t="s">
+        <v>155</v>
+      </c>
+      <c r="C11" s="28">
+        <v>691213710002</v>
+      </c>
+      <c r="D11" s="25" t="s">
+        <v>65</v>
+      </c>
+      <c r="E11" s="15" t="s">
+        <v>185</v>
+      </c>
+      <c r="F11" s="25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="26" t="s">
+        <v>156</v>
+      </c>
+      <c r="B12" s="25" t="s">
+        <v>157</v>
+      </c>
+      <c r="C12" s="28">
+        <v>691213710003</v>
+      </c>
+      <c r="D12" s="25" t="s">
+        <v>158</v>
+      </c>
+      <c r="E12" s="15" t="s">
+        <v>186</v>
+      </c>
+      <c r="F12" s="25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="26" t="s">
+        <v>126</v>
+      </c>
+      <c r="B13" s="25" t="s">
+        <v>127</v>
+      </c>
+      <c r="C13" s="28" t="s">
+        <v>128</v>
+      </c>
+      <c r="D13" s="25" t="s">
+        <v>129</v>
+      </c>
+      <c r="E13" s="15" t="s">
+        <v>187</v>
+      </c>
+      <c r="F13" s="25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="26" t="s">
+        <v>130</v>
+      </c>
+      <c r="B14" s="25" t="s">
+        <v>131</v>
+      </c>
+      <c r="C14" s="28" t="s">
+        <v>132</v>
+      </c>
+      <c r="D14" s="25" t="s">
+        <v>133</v>
+      </c>
+      <c r="E14" s="15" t="s">
+        <v>188</v>
+      </c>
+      <c r="F14" s="25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="26" t="s">
+        <v>68</v>
+      </c>
+      <c r="B15" s="25" t="s">
+        <v>61</v>
+      </c>
+      <c r="C15" s="25" t="s">
+        <v>62</v>
+      </c>
+      <c r="D15" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="E15" s="16" t="s">
         <v>63</v>
       </c>
-      <c r="B9" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="C9" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="D9" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="E9" s="20" t="s">
-        <v>24</v>
-      </c>
-      <c r="F9" s="14">
+      <c r="F15" s="27">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" s="13" customFormat="1" ht="29.4" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="26" t="s">
+        <v>69</v>
+      </c>
+      <c r="B16" s="25" t="s">
+        <v>70</v>
+      </c>
+      <c r="C16" s="28" t="s">
+        <v>75</v>
+      </c>
+      <c r="D16" s="25" t="s">
+        <v>76</v>
+      </c>
+      <c r="E16" s="15" t="s">
+        <v>189</v>
+      </c>
+      <c r="F16" s="25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A17" s="26" t="s">
+        <v>81</v>
+      </c>
+      <c r="B17" s="25" t="s">
+        <v>82</v>
+      </c>
+      <c r="C17" s="28" t="s">
+        <v>83</v>
+      </c>
+      <c r="D17" s="25" t="s">
+        <v>80</v>
+      </c>
+      <c r="E17" s="15" t="s">
+        <v>190</v>
+      </c>
+      <c r="F17" s="25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="26" t="s">
+        <v>145</v>
+      </c>
+      <c r="B18" s="25" t="s">
+        <v>48</v>
+      </c>
+      <c r="C18" s="29" t="s">
+        <v>29</v>
+      </c>
+      <c r="D18" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="E18" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="F18" s="27">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="26" t="s">
+        <v>104</v>
+      </c>
+      <c r="B19" s="25" t="s">
+        <v>105</v>
+      </c>
+      <c r="C19" s="28" t="s">
+        <v>106</v>
+      </c>
+      <c r="D19" s="25" t="s">
+        <v>80</v>
+      </c>
+      <c r="E19" s="15" t="s">
+        <v>191</v>
+      </c>
+      <c r="F19" s="25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="26" t="s">
+        <v>114</v>
+      </c>
+      <c r="B20" s="25" t="s">
+        <v>115</v>
+      </c>
+      <c r="C20" s="28" t="s">
+        <v>116</v>
+      </c>
+      <c r="D20" s="25" t="s">
+        <v>80</v>
+      </c>
+      <c r="E20" s="15" t="s">
+        <v>192</v>
+      </c>
+      <c r="F20" s="25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A21" s="26" t="s">
+        <v>120</v>
+      </c>
+      <c r="B21" s="25" t="s">
+        <v>121</v>
+      </c>
+      <c r="C21" s="28" t="s">
+        <v>122</v>
+      </c>
+      <c r="D21" s="25" t="s">
+        <v>80</v>
+      </c>
+      <c r="E21" s="15" t="s">
+        <v>193</v>
+      </c>
+      <c r="F21" s="25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="26" t="s">
+        <v>87</v>
+      </c>
+      <c r="B22" s="29" t="s">
+        <v>182</v>
+      </c>
+      <c r="C22" s="29" t="s">
+        <v>183</v>
+      </c>
+      <c r="D22" s="25" t="s">
+        <v>80</v>
+      </c>
+      <c r="E22" s="14" t="s">
+        <v>194</v>
+      </c>
+      <c r="F22" s="27">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="26" t="s">
+        <v>77</v>
+      </c>
+      <c r="B23" s="25" t="s">
+        <v>78</v>
+      </c>
+      <c r="C23" s="28" t="s">
+        <v>79</v>
+      </c>
+      <c r="D23" s="25" t="s">
+        <v>80</v>
+      </c>
+      <c r="E23" s="15" t="s">
+        <v>195</v>
+      </c>
+      <c r="F23" s="25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A24" s="26" t="s">
+        <v>94</v>
+      </c>
+      <c r="B24" s="25" t="s">
+        <v>95</v>
+      </c>
+      <c r="C24" s="28" t="s">
+        <v>96</v>
+      </c>
+      <c r="D24" s="25" t="s">
+        <v>80</v>
+      </c>
+      <c r="E24" s="15" t="s">
+        <v>196</v>
+      </c>
+      <c r="F24" s="25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="26" t="s">
+        <v>102</v>
+      </c>
+      <c r="B25" s="25" t="s">
+        <v>103</v>
+      </c>
+      <c r="C25" s="28" t="s">
+        <v>217</v>
+      </c>
+      <c r="D25" s="25" t="s">
+        <v>17</v>
+      </c>
+      <c r="E25" s="15" t="s">
+        <v>222</v>
+      </c>
+      <c r="F25" s="25">
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="19" t="s">
+    <row r="26" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A26" s="26" t="s">
+        <v>134</v>
+      </c>
+      <c r="B26" s="25" t="s">
+        <v>135</v>
+      </c>
+      <c r="C26" s="28" t="s">
+        <v>136</v>
+      </c>
+      <c r="D26" s="25" t="s">
+        <v>80</v>
+      </c>
+      <c r="E26" s="15" t="s">
+        <v>197</v>
+      </c>
+      <c r="F26" s="25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="26" t="s">
+        <v>84</v>
+      </c>
+      <c r="B27" s="25" t="s">
+        <v>85</v>
+      </c>
+      <c r="C27" s="28" t="s">
+        <v>86</v>
+      </c>
+      <c r="D27" s="25" t="s">
+        <v>80</v>
+      </c>
+      <c r="E27" s="15" t="s">
+        <v>198</v>
+      </c>
+      <c r="F27" s="25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="26" t="s">
+        <v>99</v>
+      </c>
+      <c r="B28" s="25" t="s">
+        <v>100</v>
+      </c>
+      <c r="C28" s="28" t="s">
+        <v>101</v>
+      </c>
+      <c r="D28" s="25" t="s">
+        <v>80</v>
+      </c>
+      <c r="E28" s="15" t="s">
+        <v>199</v>
+      </c>
+      <c r="F28" s="25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A29" s="26" t="s">
+        <v>66</v>
+      </c>
+      <c r="B29" s="29" t="s">
+        <v>55</v>
+      </c>
+      <c r="C29" s="29" t="s">
+        <v>54</v>
+      </c>
+      <c r="D29" s="25" t="s">
+        <v>56</v>
+      </c>
+      <c r="E29" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="F29" s="27">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" s="26" t="s">
+        <v>159</v>
+      </c>
+      <c r="B30" s="25" t="s">
+        <v>160</v>
+      </c>
+      <c r="C30" s="28" t="s">
+        <v>161</v>
+      </c>
+      <c r="D30" s="25" t="s">
+        <v>80</v>
+      </c>
+      <c r="E30" s="15" t="s">
+        <v>200</v>
+      </c>
+      <c r="F30" s="25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" s="26" t="s">
+        <v>123</v>
+      </c>
+      <c r="B31" s="25" t="s">
+        <v>124</v>
+      </c>
+      <c r="C31" s="28" t="s">
+        <v>125</v>
+      </c>
+      <c r="D31" s="25" t="s">
+        <v>80</v>
+      </c>
+      <c r="E31" s="15" t="s">
+        <v>201</v>
+      </c>
+      <c r="F31" s="25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A32" s="26" t="s">
+        <v>146</v>
+      </c>
+      <c r="B32" s="25" t="s">
+        <v>147</v>
+      </c>
+      <c r="C32" s="28" t="s">
+        <v>148</v>
+      </c>
+      <c r="D32" s="25" t="s">
+        <v>140</v>
+      </c>
+      <c r="E32" s="15" t="s">
+        <v>202</v>
+      </c>
+      <c r="F32" s="25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A33" s="26" t="s">
+        <v>137</v>
+      </c>
+      <c r="B33" s="25" t="s">
+        <v>138</v>
+      </c>
+      <c r="C33" s="28" t="s">
+        <v>139</v>
+      </c>
+      <c r="D33" s="25" t="s">
+        <v>140</v>
+      </c>
+      <c r="E33" s="15" t="s">
+        <v>203</v>
+      </c>
+      <c r="F33" s="25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" s="26" t="s">
+        <v>107</v>
+      </c>
+      <c r="B34" s="25" t="s">
+        <v>108</v>
+      </c>
+      <c r="C34" s="28" t="s">
+        <v>109</v>
+      </c>
+      <c r="D34" s="25" t="s">
+        <v>56</v>
+      </c>
+      <c r="E34" s="15" t="s">
+        <v>204</v>
+      </c>
+      <c r="F34" s="25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" s="26" t="s">
+        <v>117</v>
+      </c>
+      <c r="B35" s="25" t="s">
+        <v>118</v>
+      </c>
+      <c r="C35" s="28" t="s">
+        <v>119</v>
+      </c>
+      <c r="D35" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="E35" s="15" t="s">
+        <v>205</v>
+      </c>
+      <c r="F35" s="25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" s="26" t="s">
+        <v>88</v>
+      </c>
+      <c r="B36" s="25" t="s">
+        <v>184</v>
+      </c>
+      <c r="C36" s="28" t="s">
+        <v>89</v>
+      </c>
+      <c r="D36" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="E36" s="15" t="s">
+        <v>206</v>
+      </c>
+      <c r="F36" s="25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A37" s="26" t="s">
+        <v>180</v>
+      </c>
+      <c r="B37" s="25" t="s">
+        <v>207</v>
+      </c>
+      <c r="C37" s="25" t="s">
+        <v>53</v>
+      </c>
+      <c r="D37" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="E37" s="14" t="s">
+        <v>208</v>
+      </c>
+      <c r="F37" s="27">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" s="26" t="s">
+        <v>97</v>
+      </c>
+      <c r="B38" s="25" t="s">
+        <v>98</v>
+      </c>
+      <c r="C38" s="28" t="s">
+        <v>218</v>
+      </c>
+      <c r="D38" s="25" t="s">
+        <v>219</v>
+      </c>
+      <c r="E38" s="15" t="s">
+        <v>223</v>
+      </c>
+      <c r="F38" s="25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" s="26" t="s">
+        <v>149</v>
+      </c>
+      <c r="B39" s="25" t="s">
+        <v>227</v>
+      </c>
+      <c r="C39" s="28" t="s">
+        <v>226</v>
+      </c>
+      <c r="D39" s="25" t="s">
+        <v>144</v>
+      </c>
+      <c r="E39" s="15" t="s">
+        <v>228</v>
+      </c>
+      <c r="F39" s="25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" s="26" t="s">
+        <v>51</v>
+      </c>
+      <c r="B40" s="29" t="s">
+        <v>47</v>
+      </c>
+      <c r="C40" s="29" t="s">
+        <v>26</v>
+      </c>
+      <c r="D40" s="29" t="s">
+        <v>25</v>
+      </c>
+      <c r="E40" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="F40" s="27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41" s="26" t="s">
+        <v>110</v>
+      </c>
+      <c r="B41" s="25" t="s">
+        <v>111</v>
+      </c>
+      <c r="C41" s="28" t="s">
+        <v>112</v>
+      </c>
+      <c r="D41" s="25" t="s">
+        <v>113</v>
+      </c>
+      <c r="E41" s="15" t="s">
+        <v>209</v>
+      </c>
+      <c r="F41" s="25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42" s="26" t="s">
+        <v>52</v>
+      </c>
+      <c r="B42" s="25" t="s">
+        <v>46</v>
+      </c>
+      <c r="C42" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="D42" s="25" t="s">
+        <v>17</v>
+      </c>
+      <c r="E42" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="F42" s="27">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A43" s="26" t="s">
+        <v>90</v>
+      </c>
+      <c r="B43" s="25" t="s">
+        <v>91</v>
+      </c>
+      <c r="C43" s="28" t="s">
+        <v>92</v>
+      </c>
+      <c r="D43" s="25" t="s">
+        <v>93</v>
+      </c>
+      <c r="E43" s="15" t="s">
+        <v>210</v>
+      </c>
+      <c r="F43" s="25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44" s="26" t="s">
+        <v>152</v>
+      </c>
+      <c r="B44" s="25" t="s">
+        <v>153</v>
+      </c>
+      <c r="C44" s="28" t="s">
+        <v>220</v>
+      </c>
+      <c r="D44" s="25" t="s">
+        <v>93</v>
+      </c>
+      <c r="E44" s="15" t="s">
+        <v>224</v>
+      </c>
+      <c r="F44" s="25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45" s="26" t="s">
+        <v>150</v>
+      </c>
+      <c r="B45" s="25" t="s">
+        <v>151</v>
+      </c>
+      <c r="C45" s="28" t="s">
+        <v>221</v>
+      </c>
+      <c r="D45" s="25" t="s">
+        <v>219</v>
+      </c>
+      <c r="E45" s="15" t="s">
+        <v>225</v>
+      </c>
+      <c r="F45" s="25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="26" t="s">
+        <v>31</v>
+      </c>
+      <c r="B46" s="25" t="s">
+        <v>32</v>
+      </c>
+      <c r="C46" s="25" t="s">
+        <v>34</v>
+      </c>
+      <c r="D46" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="E46" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="F46" s="27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A47" s="26" t="s">
+        <v>141</v>
+      </c>
+      <c r="B47" s="25" t="s">
+        <v>142</v>
+      </c>
+      <c r="C47" s="28" t="s">
+        <v>143</v>
+      </c>
+      <c r="D47" s="25" t="s">
+        <v>144</v>
+      </c>
+      <c r="E47" s="15" t="s">
+        <v>211</v>
+      </c>
+      <c r="F47" s="25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A48" s="26" t="s">
+        <v>176</v>
+      </c>
+      <c r="B48" s="25" t="s">
+        <v>49</v>
+      </c>
+      <c r="C48" s="25" t="s">
+        <v>41</v>
+      </c>
+      <c r="D48" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="E48" s="14" t="s">
+        <v>212</v>
+      </c>
+      <c r="F48" s="27">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A49" s="26" t="s">
+        <v>164</v>
+      </c>
+      <c r="B49" s="25" t="s">
+        <v>165</v>
+      </c>
+      <c r="C49" s="28" t="s">
+        <v>166</v>
+      </c>
+      <c r="D49" s="25" t="s">
+        <v>39</v>
+      </c>
+      <c r="E49" s="15" t="s">
+        <v>167</v>
+      </c>
+      <c r="F49" s="25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A50" s="26" t="s">
+        <v>168</v>
+      </c>
+      <c r="B50" s="25" t="s">
+        <v>169</v>
+      </c>
+      <c r="C50" s="28" t="s">
+        <v>170</v>
+      </c>
+      <c r="D50" s="25" t="s">
+        <v>171</v>
+      </c>
+      <c r="E50" s="15" t="s">
+        <v>213</v>
+      </c>
+      <c r="F50" s="25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A51" s="26" t="s">
         <v>67</v>
       </c>
-      <c r="B10" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="C10" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="D10" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="E10" s="20" t="s">
-        <v>27</v>
-      </c>
-      <c r="F10" s="14">
+      <c r="B51" s="25" t="s">
+        <v>71</v>
+      </c>
+      <c r="C51" s="28" t="s">
+        <v>72</v>
+      </c>
+      <c r="D51" s="25" t="s">
+        <v>73</v>
+      </c>
+      <c r="E51" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="F51" s="25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A52" s="26" t="s">
+        <v>37</v>
+      </c>
+      <c r="B52" s="25" t="s">
+        <v>38</v>
+      </c>
+      <c r="C52" s="25" t="s">
+        <v>36</v>
+      </c>
+      <c r="D52" s="25" t="s">
+        <v>39</v>
+      </c>
+      <c r="E52" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="F52" s="27">
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="19" t="s">
-        <v>157</v>
-      </c>
-      <c r="B11" s="13" t="s">
-        <v>158</v>
-      </c>
-      <c r="C11" s="17">
-        <v>691213710002</v>
-      </c>
-      <c r="D11" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="E11" s="21" t="s">
-        <v>188</v>
-      </c>
-      <c r="F11" s="13">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A53" s="26" t="s">
+        <v>58</v>
+      </c>
+      <c r="B53" s="25" t="s">
+        <v>177</v>
+      </c>
+      <c r="C53" s="28" t="s">
+        <v>178</v>
+      </c>
+      <c r="D53" s="25" t="s">
+        <v>39</v>
+      </c>
+      <c r="E53" s="15" t="s">
+        <v>179</v>
+      </c>
+      <c r="F53" s="25">
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="19" t="s">
-        <v>159</v>
-      </c>
-      <c r="B12" s="13" t="s">
-        <v>160</v>
-      </c>
-      <c r="C12" s="17">
-        <v>691213710003</v>
-      </c>
-      <c r="D12" s="13" t="s">
-        <v>161</v>
-      </c>
-      <c r="E12" s="21" t="s">
-        <v>189</v>
-      </c>
-      <c r="F12" s="13">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A54" s="26" t="s">
+        <v>162</v>
+      </c>
+      <c r="B54" s="25" t="s">
+        <v>216</v>
+      </c>
+      <c r="C54" s="28" t="s">
+        <v>163</v>
+      </c>
+      <c r="D54" s="25" t="s">
+        <v>57</v>
+      </c>
+      <c r="E54" s="15" t="s">
+        <v>214</v>
+      </c>
+      <c r="F54" s="25">
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="19" t="s">
-        <v>129</v>
-      </c>
-      <c r="B13" s="13" t="s">
-        <v>130</v>
-      </c>
-      <c r="C13" s="17" t="s">
-        <v>131</v>
-      </c>
-      <c r="D13" s="13" t="s">
-        <v>132</v>
-      </c>
-      <c r="E13" s="21" t="s">
-        <v>190</v>
-      </c>
-      <c r="F13" s="13">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A55" s="26" t="s">
+        <v>172</v>
+      </c>
+      <c r="B55" s="25" t="s">
+        <v>173</v>
+      </c>
+      <c r="C55" s="28" t="s">
+        <v>174</v>
+      </c>
+      <c r="D55" s="25" t="s">
+        <v>175</v>
+      </c>
+      <c r="E55" s="15" t="s">
+        <v>215</v>
+      </c>
+      <c r="F55" s="25">
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="19" t="s">
-        <v>133</v>
-      </c>
-      <c r="B14" s="13" t="s">
-        <v>134</v>
-      </c>
-      <c r="C14" s="17" t="s">
-        <v>135</v>
-      </c>
-      <c r="D14" s="13" t="s">
-        <v>136</v>
-      </c>
-      <c r="E14" s="21" t="s">
-        <v>191</v>
-      </c>
-      <c r="F14" s="13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="19" t="s">
-        <v>71</v>
-      </c>
-      <c r="B15" s="13" t="s">
-        <v>64</v>
-      </c>
-      <c r="C15" s="13" t="s">
-        <v>65</v>
-      </c>
-      <c r="D15" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="E15" s="22" t="s">
-        <v>66</v>
-      </c>
-      <c r="F15" s="14">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" s="18" customFormat="1" ht="29.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="19" t="s">
-        <v>72</v>
-      </c>
-      <c r="B16" s="13" t="s">
-        <v>73</v>
-      </c>
-      <c r="C16" s="17" t="s">
-        <v>78</v>
-      </c>
-      <c r="D16" s="13" t="s">
-        <v>79</v>
-      </c>
-      <c r="E16" s="21" t="s">
-        <v>192</v>
-      </c>
-      <c r="F16" s="13">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A17" s="19" t="s">
-        <v>84</v>
-      </c>
-      <c r="B17" s="13" t="s">
-        <v>85</v>
-      </c>
-      <c r="C17" s="17" t="s">
-        <v>86</v>
-      </c>
-      <c r="D17" s="13" t="s">
-        <v>83</v>
-      </c>
-      <c r="E17" s="21" t="s">
-        <v>193</v>
-      </c>
-      <c r="F17" s="13">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="19" t="s">
-        <v>148</v>
-      </c>
-      <c r="B18" s="13" t="s">
-        <v>51</v>
-      </c>
-      <c r="C18" s="15" t="s">
-        <v>32</v>
-      </c>
-      <c r="D18" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="E18" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="F18" s="14">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="19" t="s">
-        <v>107</v>
-      </c>
-      <c r="B19" s="13" t="s">
-        <v>108</v>
-      </c>
-      <c r="C19" s="17" t="s">
-        <v>109</v>
-      </c>
-      <c r="D19" s="13" t="s">
-        <v>83</v>
-      </c>
-      <c r="E19" s="21" t="s">
-        <v>194</v>
-      </c>
-      <c r="F19" s="13">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="19" t="s">
-        <v>117</v>
-      </c>
-      <c r="B20" s="13" t="s">
-        <v>118</v>
-      </c>
-      <c r="C20" s="17" t="s">
-        <v>119</v>
-      </c>
-      <c r="D20" s="13" t="s">
-        <v>83</v>
-      </c>
-      <c r="E20" s="21" t="s">
-        <v>195</v>
-      </c>
-      <c r="F20" s="13">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A21" s="19" t="s">
-        <v>123</v>
-      </c>
-      <c r="B21" s="13" t="s">
-        <v>124</v>
-      </c>
-      <c r="C21" s="17" t="s">
-        <v>125</v>
-      </c>
-      <c r="D21" s="13" t="s">
-        <v>83</v>
-      </c>
-      <c r="E21" s="21" t="s">
-        <v>196</v>
-      </c>
-      <c r="F21" s="13">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="19" t="s">
-        <v>90</v>
-      </c>
-      <c r="B22" s="15" t="s">
-        <v>185</v>
-      </c>
-      <c r="C22" s="15" t="s">
-        <v>186</v>
-      </c>
-      <c r="D22" s="13" t="s">
-        <v>83</v>
-      </c>
-      <c r="E22" s="20" t="s">
-        <v>197</v>
-      </c>
-      <c r="F22" s="14">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="19" t="s">
-        <v>80</v>
-      </c>
-      <c r="B23" s="13" t="s">
-        <v>81</v>
-      </c>
-      <c r="C23" s="17" t="s">
-        <v>82</v>
-      </c>
-      <c r="D23" s="13" t="s">
-        <v>83</v>
-      </c>
-      <c r="E23" s="21" t="s">
-        <v>198</v>
-      </c>
-      <c r="F23" s="13">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A24" s="19" t="s">
-        <v>97</v>
-      </c>
-      <c r="B24" s="13" t="s">
-        <v>98</v>
-      </c>
-      <c r="C24" s="17" t="s">
-        <v>99</v>
-      </c>
-      <c r="D24" s="13" t="s">
-        <v>83</v>
-      </c>
-      <c r="E24" s="21" t="s">
-        <v>199</v>
-      </c>
-      <c r="F24" s="13">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="19" t="s">
-        <v>105</v>
-      </c>
-      <c r="B25" s="13" t="s">
-        <v>106</v>
-      </c>
-      <c r="C25" s="17" t="s">
-        <v>220</v>
-      </c>
-      <c r="D25" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="E25" s="21" t="s">
-        <v>225</v>
-      </c>
-      <c r="F25" s="13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A26" s="19" t="s">
-        <v>137</v>
-      </c>
-      <c r="B26" s="13" t="s">
-        <v>138</v>
-      </c>
-      <c r="C26" s="17" t="s">
-        <v>139</v>
-      </c>
-      <c r="D26" s="13" t="s">
-        <v>83</v>
-      </c>
-      <c r="E26" s="21" t="s">
-        <v>200</v>
-      </c>
-      <c r="F26" s="13">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="19" t="s">
-        <v>87</v>
-      </c>
-      <c r="B27" s="13" t="s">
-        <v>88</v>
-      </c>
-      <c r="C27" s="17" t="s">
-        <v>89</v>
-      </c>
-      <c r="D27" s="13" t="s">
-        <v>83</v>
-      </c>
-      <c r="E27" s="21" t="s">
-        <v>201</v>
-      </c>
-      <c r="F27" s="13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="19" t="s">
-        <v>102</v>
-      </c>
-      <c r="B28" s="13" t="s">
-        <v>103</v>
-      </c>
-      <c r="C28" s="17" t="s">
-        <v>104</v>
-      </c>
-      <c r="D28" s="13" t="s">
-        <v>83</v>
-      </c>
-      <c r="E28" s="21" t="s">
-        <v>202</v>
-      </c>
-      <c r="F28" s="13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A29" s="19" t="s">
-        <v>69</v>
-      </c>
-      <c r="B29" s="15" t="s">
-        <v>58</v>
-      </c>
-      <c r="C29" s="15" t="s">
-        <v>57</v>
-      </c>
-      <c r="D29" s="13" t="s">
-        <v>59</v>
-      </c>
-      <c r="E29" s="20" t="s">
-        <v>62</v>
-      </c>
-      <c r="F29" s="14">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="19" t="s">
-        <v>162</v>
-      </c>
-      <c r="B30" s="13" t="s">
-        <v>163</v>
-      </c>
-      <c r="C30" s="17" t="s">
-        <v>164</v>
-      </c>
-      <c r="D30" s="13" t="s">
-        <v>83</v>
-      </c>
-      <c r="E30" s="21" t="s">
-        <v>203</v>
-      </c>
-      <c r="F30" s="13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="19" t="s">
-        <v>126</v>
-      </c>
-      <c r="B31" s="13" t="s">
-        <v>127</v>
-      </c>
-      <c r="C31" s="17" t="s">
-        <v>128</v>
-      </c>
-      <c r="D31" s="13" t="s">
-        <v>83</v>
-      </c>
-      <c r="E31" s="21" t="s">
-        <v>204</v>
-      </c>
-      <c r="F31" s="13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="19" t="s">
-        <v>149</v>
-      </c>
-      <c r="B32" s="13" t="s">
-        <v>150</v>
-      </c>
-      <c r="C32" s="17" t="s">
-        <v>151</v>
-      </c>
-      <c r="D32" s="13" t="s">
-        <v>143</v>
-      </c>
-      <c r="E32" s="21" t="s">
-        <v>205</v>
-      </c>
-      <c r="F32" s="13">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="19" t="s">
-        <v>140</v>
-      </c>
-      <c r="B33" s="13" t="s">
-        <v>141</v>
-      </c>
-      <c r="C33" s="17" t="s">
-        <v>142</v>
-      </c>
-      <c r="D33" s="13" t="s">
-        <v>143</v>
-      </c>
-      <c r="E33" s="21" t="s">
-        <v>206</v>
-      </c>
-      <c r="F33" s="13">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="19" t="s">
-        <v>110</v>
-      </c>
-      <c r="B34" s="13" t="s">
-        <v>111</v>
-      </c>
-      <c r="C34" s="17" t="s">
-        <v>112</v>
-      </c>
-      <c r="D34" s="13" t="s">
-        <v>59</v>
-      </c>
-      <c r="E34" s="21" t="s">
-        <v>207</v>
-      </c>
-      <c r="F34" s="13">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="19" t="s">
-        <v>120</v>
-      </c>
-      <c r="B35" s="13" t="s">
-        <v>121</v>
-      </c>
-      <c r="C35" s="17" t="s">
-        <v>122</v>
-      </c>
-      <c r="D35" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="E35" s="21" t="s">
-        <v>208</v>
-      </c>
-      <c r="F35" s="13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="19" t="s">
-        <v>91</v>
-      </c>
-      <c r="B36" s="13" t="s">
-        <v>187</v>
-      </c>
-      <c r="C36" s="17" t="s">
-        <v>92</v>
-      </c>
-      <c r="D36" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="E36" s="21" t="s">
-        <v>209</v>
-      </c>
-      <c r="F36" s="13">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A37" s="19" t="s">
-        <v>183</v>
-      </c>
-      <c r="B37" s="13" t="s">
-        <v>210</v>
-      </c>
-      <c r="C37" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="D37" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="E37" s="20" t="s">
-        <v>211</v>
-      </c>
-      <c r="F37" s="14">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" s="19" t="s">
-        <v>100</v>
-      </c>
-      <c r="B38" s="13" t="s">
-        <v>101</v>
-      </c>
-      <c r="C38" s="17" t="s">
-        <v>221</v>
-      </c>
-      <c r="D38" s="13" t="s">
-        <v>222</v>
-      </c>
-      <c r="E38" s="21" t="s">
-        <v>226</v>
-      </c>
-      <c r="F38" s="13">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" s="19" t="s">
-        <v>152</v>
-      </c>
-      <c r="B39" s="13" t="s">
-        <v>230</v>
-      </c>
-      <c r="C39" s="17" t="s">
-        <v>229</v>
-      </c>
-      <c r="D39" s="13" t="s">
-        <v>147</v>
-      </c>
-      <c r="E39" s="31" t="s">
-        <v>231</v>
-      </c>
-      <c r="F39" s="13">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" s="19" t="s">
-        <v>54</v>
-      </c>
-      <c r="B40" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="C40" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="D40" s="15" t="s">
-        <v>28</v>
-      </c>
-      <c r="E40" s="20" t="s">
-        <v>30</v>
-      </c>
-      <c r="F40" s="14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41" s="19" t="s">
-        <v>113</v>
-      </c>
-      <c r="B41" s="13" t="s">
-        <v>114</v>
-      </c>
-      <c r="C41" s="17" t="s">
-        <v>115</v>
-      </c>
-      <c r="D41" s="13" t="s">
-        <v>116</v>
-      </c>
-      <c r="E41" s="21" t="s">
-        <v>212</v>
-      </c>
-      <c r="F41" s="13">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A42" s="19" t="s">
-        <v>55</v>
-      </c>
-      <c r="B42" s="13" t="s">
-        <v>49</v>
-      </c>
-      <c r="C42" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="D42" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="E42" s="20" t="s">
-        <v>19</v>
-      </c>
-      <c r="F42" s="14">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A43" s="19" t="s">
-        <v>93</v>
-      </c>
-      <c r="B43" s="13" t="s">
-        <v>94</v>
-      </c>
-      <c r="C43" s="17" t="s">
-        <v>95</v>
-      </c>
-      <c r="D43" s="13" t="s">
-        <v>96</v>
-      </c>
-      <c r="E43" s="21" t="s">
-        <v>213</v>
-      </c>
-      <c r="F43" s="13">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A44" s="19" t="s">
-        <v>155</v>
-      </c>
-      <c r="B44" s="13" t="s">
-        <v>156</v>
-      </c>
-      <c r="C44" s="17" t="s">
-        <v>223</v>
-      </c>
-      <c r="D44" s="13" t="s">
-        <v>96</v>
-      </c>
-      <c r="E44" s="21" t="s">
-        <v>227</v>
-      </c>
-      <c r="F44" s="13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A45" s="19" t="s">
-        <v>153</v>
-      </c>
-      <c r="B45" s="13" t="s">
-        <v>154</v>
-      </c>
-      <c r="C45" s="17" t="s">
-        <v>224</v>
-      </c>
-      <c r="D45" s="13" t="s">
-        <v>222</v>
-      </c>
-      <c r="E45" s="21" t="s">
-        <v>228</v>
-      </c>
-      <c r="F45" s="13">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="19" t="s">
-        <v>34</v>
-      </c>
-      <c r="B46" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="C46" s="13" t="s">
-        <v>37</v>
-      </c>
-      <c r="D46" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="E46" s="20" t="s">
-        <v>38</v>
-      </c>
-      <c r="F46" s="14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A47" s="19" t="s">
-        <v>144</v>
-      </c>
-      <c r="B47" s="13" t="s">
-        <v>145</v>
-      </c>
-      <c r="C47" s="17" t="s">
-        <v>146</v>
-      </c>
-      <c r="D47" s="13" t="s">
-        <v>147</v>
-      </c>
-      <c r="E47" s="21" t="s">
-        <v>214</v>
-      </c>
-      <c r="F47" s="13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A48" s="19" t="s">
-        <v>179</v>
-      </c>
-      <c r="B48" s="13" t="s">
-        <v>52</v>
-      </c>
-      <c r="C48" s="13" t="s">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A56" s="26" t="s">
+        <v>42</v>
+      </c>
+      <c r="B56" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="C56" s="25" t="s">
         <v>44</v>
       </c>
-      <c r="D48" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="E48" s="20" t="s">
-        <v>215</v>
-      </c>
-      <c r="F48" s="14">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A49" s="19" t="s">
-        <v>167</v>
-      </c>
-      <c r="B49" s="13" t="s">
-        <v>168</v>
-      </c>
-      <c r="C49" s="17" t="s">
-        <v>169</v>
-      </c>
-      <c r="D49" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="E49" s="21" t="s">
-        <v>170</v>
-      </c>
-      <c r="F49" s="13">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A50" s="19" t="s">
-        <v>171</v>
-      </c>
-      <c r="B50" s="13" t="s">
-        <v>172</v>
-      </c>
-      <c r="C50" s="17" t="s">
-        <v>173</v>
-      </c>
-      <c r="D50" s="13" t="s">
-        <v>174</v>
-      </c>
-      <c r="E50" s="21" t="s">
-        <v>216</v>
-      </c>
-      <c r="F50" s="13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A51" s="19" t="s">
-        <v>70</v>
-      </c>
-      <c r="B51" s="13" t="s">
-        <v>74</v>
-      </c>
-      <c r="C51" s="17" t="s">
-        <v>75</v>
-      </c>
-      <c r="D51" s="13" t="s">
-        <v>76</v>
-      </c>
-      <c r="E51" s="21" t="s">
-        <v>77</v>
-      </c>
-      <c r="F51" s="13">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A52" s="19" t="s">
-        <v>40</v>
-      </c>
-      <c r="B52" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="C52" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="D52" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="E52" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="F52" s="14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A53" s="19" t="s">
-        <v>61</v>
-      </c>
-      <c r="B53" s="13" t="s">
-        <v>180</v>
-      </c>
-      <c r="C53" s="17" t="s">
-        <v>181</v>
-      </c>
-      <c r="D53" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="E53" s="21" t="s">
-        <v>182</v>
-      </c>
-      <c r="F53" s="13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A54" s="19" t="s">
-        <v>165</v>
-      </c>
-      <c r="B54" s="13" t="s">
-        <v>219</v>
-      </c>
-      <c r="C54" s="17" t="s">
-        <v>166</v>
-      </c>
-      <c r="D54" s="13" t="s">
-        <v>60</v>
-      </c>
-      <c r="E54" s="21" t="s">
-        <v>217</v>
-      </c>
-      <c r="F54" s="13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A55" s="19" t="s">
-        <v>175</v>
-      </c>
-      <c r="B55" s="13" t="s">
-        <v>176</v>
-      </c>
-      <c r="C55" s="17" t="s">
-        <v>177</v>
-      </c>
-      <c r="D55" s="13" t="s">
-        <v>178</v>
-      </c>
-      <c r="E55" s="21" t="s">
-        <v>218</v>
-      </c>
-      <c r="F55" s="13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A56" s="19" t="s">
+      <c r="D56" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="E56" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="B56" s="13" t="s">
-        <v>46</v>
-      </c>
-      <c r="C56" s="13" t="s">
-        <v>47</v>
-      </c>
-      <c r="D56" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="E56" s="20" t="s">
-        <v>48</v>
-      </c>
-      <c r="F56" s="16">
+      <c r="F56" s="30">
         <v>1</v>
       </c>
     </row>
@@ -2953,45 +2942,44 @@
     <mergeCell ref="D6:F6"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="E9" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="E18" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="E10" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="E51" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="E15" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="E16" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="E17" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="E19" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="E20" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
-    <hyperlink ref="E21" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
-    <hyperlink ref="E22" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
-    <hyperlink ref="E23" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
-    <hyperlink ref="E24" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
-    <hyperlink ref="E26" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
-    <hyperlink ref="E27" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
-    <hyperlink ref="E28" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
-    <hyperlink ref="E29" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
-    <hyperlink ref="E30" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
-    <hyperlink ref="E31" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
-    <hyperlink ref="E32" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
-    <hyperlink ref="E33" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
-    <hyperlink ref="E34" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
-    <hyperlink ref="E35" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
-    <hyperlink ref="E36" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
-    <hyperlink ref="E37" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
-    <hyperlink ref="E40" r:id="rId26" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
-    <hyperlink ref="E41" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
-    <hyperlink ref="E42" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
-    <hyperlink ref="E46" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
-    <hyperlink ref="E47" r:id="rId30" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
-    <hyperlink ref="E48" r:id="rId31" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
-    <hyperlink ref="E49" r:id="rId32" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
-    <hyperlink ref="E50" r:id="rId33" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
-    <hyperlink ref="E54" r:id="rId34" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
-    <hyperlink ref="E43" r:id="rId35" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
-    <hyperlink ref="E39" r:id="rId36" xr:uid="{BCAA706E-A458-4DA7-9B07-DBD2AB7D3535}"/>
+    <hyperlink ref="E18" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="E10" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="E51" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="E15" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="E16" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="E17" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="E19" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="E20" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="E21" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="E22" r:id="rId10" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="E23" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="E24" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="E26" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="E27" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="E28" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="E29" r:id="rId16" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="E30" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="E31" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="E32" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="E33" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
+    <hyperlink ref="E34" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
+    <hyperlink ref="E35" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
+    <hyperlink ref="E36" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
+    <hyperlink ref="E37" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
+    <hyperlink ref="E40" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
+    <hyperlink ref="E41" r:id="rId26" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
+    <hyperlink ref="E42" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
+    <hyperlink ref="E46" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
+    <hyperlink ref="E47" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
+    <hyperlink ref="E48" r:id="rId30" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
+    <hyperlink ref="E49" r:id="rId31" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
+    <hyperlink ref="E50" r:id="rId32" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
+    <hyperlink ref="E54" r:id="rId33" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
+    <hyperlink ref="E43" r:id="rId34" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
+    <hyperlink ref="E39" r:id="rId35" xr:uid="{BCAA706E-A458-4DA7-9B07-DBD2AB7D3535}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId37"/>
-  <drawing r:id="rId38"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId36"/>
+  <drawing r:id="rId37"/>
 </worksheet>
 </file>
</xml_diff>